<commit_message>
Rewrite to cog done
</commit_message>
<xml_diff>
--- a/config/generator/card_list.xlsx
+++ b/config/generator/card_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\670264231\CLionProjects\dominion-setup-counter\config\generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E837FC0E-7722-483B-9F53-E95DC4694F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123F7E14-E665-4728-A261-C964B89141BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4845" yWindow="4245" windowWidth="21600" windowHeight="11505" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kingdom" sheetId="1" r:id="rId1"/>
@@ -13727,7 +13727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D52C678-4E61-407F-A442-FC0A28FC9EC1}">
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -17104,7 +17104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC0FE835-BF2D-4255-A7C9-5755E3DA90BF}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>